<commit_message>
update: user bulk upload
</commit_message>
<xml_diff>
--- a/public/user_bulk_upload.xlsx
+++ b/public/user_bulk_upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <r>
       <rPr>
@@ -70,22 +70,82 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Gender </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Designation </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Phone </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
   </si>
 </sst>
 </file>
@@ -95,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,6 +193,14 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,10 +458,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -403,7 +471,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,11 +495,6 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>